<commit_message>
added clear_teacher to modulus
</commit_message>
<xml_diff>
--- a/db_info/projeto2024.xlsx
+++ b/db_info/projeto2024.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="440">
   <si>
     <t xml:space="preserve">code</t>
   </si>
@@ -2118,10 +2118,10 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F108" activeCellId="0" sqref="F108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.4921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5197,7 +5197,9 @@
       <c r="E84" s="49" t="s">
         <v>346</v>
       </c>
-      <c r="F84" s="36"/>
+      <c r="F84" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="G84" s="36"/>
       <c r="H84" s="50"/>
       <c r="I84" s="50"/>
@@ -5877,7 +5879,9 @@
       <c r="E104" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="F104" s="5"/>
+      <c r="F104" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="G104" s="8"/>
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
@@ -5937,7 +5941,9 @@
       <c r="E106" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="F106" s="10"/>
+      <c r="F106" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="G106" s="12"/>
       <c r="H106" s="10"/>
       <c r="I106" s="10"/>

</xml_diff>

<commit_message>
added get_by_code to modulus
</commit_message>
<xml_diff>
--- a/db_info/projeto2024.xlsx
+++ b/db_info/projeto2024.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="DISCIPLINAS 2024" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Planilha2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="DISCIPLINAS 2024" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Planilha2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'DISCIPLINAS 2024'!$B$2:$B$3</definedName>
@@ -1589,7 +1589,7 @@
     <numFmt numFmtId="165" formatCode="d\.m"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1640,12 +1640,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1818,7 +1812,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1951,14 +1945,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1983,31 +1969,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2023,7 +1993,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2035,59 +2005,55 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2163,8 +2129,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2173,7 +2245,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D102" activeCellId="0" sqref="D102"/>
+      <selection pane="bottomLeft" activeCell="E113" activeCellId="0" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.484375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2184,7 +2256,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="62.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.73"/>
@@ -2255,7 +2327,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J2" s="10" t="b">
+      <c r="J2" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2291,7 +2363,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J3" s="10" t="b">
+      <c r="J3" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2329,7 +2401,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J4" s="15" t="b">
+      <c r="J4" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2367,7 +2439,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J5" s="15" t="b">
+      <c r="J5" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2405,7 +2477,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J6" s="22" t="b">
+      <c r="J6" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2443,7 +2515,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J7" s="22" t="b">
+      <c r="J7" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2481,7 +2553,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J8" s="15" t="b">
+      <c r="J8" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2519,7 +2591,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J9" s="15" t="b">
+      <c r="J9" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2557,7 +2629,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J10" s="22" t="b">
+      <c r="J10" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2595,7 +2667,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J11" s="22" t="b">
+      <c r="J11" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2633,7 +2705,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J12" s="15" t="b">
+      <c r="J12" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2671,7 +2743,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J13" s="22" t="b">
+      <c r="J13" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2707,7 +2779,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J14" s="15" t="b">
+      <c r="J14" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2745,7 +2817,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J15" s="10" t="b">
+      <c r="J15" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2783,7 +2855,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J16" s="10" t="b">
+      <c r="J16" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2821,7 +2893,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J17" s="15" t="b">
+      <c r="J17" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2859,7 +2931,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J18" s="10" t="b">
+      <c r="J18" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2897,7 +2969,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J19" s="15" t="b">
+      <c r="J19" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2935,7 +3007,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J20" s="10" t="b">
+      <c r="J20" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2953,7 +3025,7 @@
       <c r="B21" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="12" t="s">
         <v>83</v>
       </c>
       <c r="D21" s="32" t="n">
@@ -2973,7 +3045,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J21" s="15" t="b">
+      <c r="J21" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3011,7 +3083,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J22" s="15" t="b">
+      <c r="J22" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3075,7 +3147,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J24" s="15" t="b">
+      <c r="J24" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3111,7 +3183,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J25" s="10" t="b">
+      <c r="J25" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3145,7 +3217,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J26" s="15" t="b">
+      <c r="J26" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3163,7 +3235,7 @@
       <c r="B27" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="6" t="s">
         <v>108</v>
       </c>
       <c r="D27" s="6" t="n">
@@ -3181,7 +3253,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J27" s="10" t="b">
+      <c r="J27" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3215,11 +3287,11 @@
         <v>1</v>
       </c>
       <c r="H28" s="6"/>
-      <c r="I28" s="10" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="10" t="b">
+      <c r="I28" s="6" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3253,11 +3325,11 @@
         <v>1</v>
       </c>
       <c r="H29" s="12"/>
-      <c r="I29" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="15" t="b">
+      <c r="I29" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3293,7 +3365,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J30" s="10" t="b">
+      <c r="J30" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3329,7 +3401,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J31" s="15" t="b">
+      <c r="J31" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3363,11 +3435,11 @@
         <v>1</v>
       </c>
       <c r="H32" s="6"/>
-      <c r="I32" s="10" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J32" s="10" t="b">
+      <c r="I32" s="6" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3401,11 +3473,11 @@
         <v>1</v>
       </c>
       <c r="H33" s="6"/>
-      <c r="I33" s="10" t="b">
+      <c r="I33" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J33" s="10" t="b">
+      <c r="J33" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3442,7 +3514,7 @@
       <c r="I34" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="J34" s="15" t="b">
+      <c r="J34" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3474,11 +3546,11 @@
         <v>1</v>
       </c>
       <c r="H35" s="6"/>
-      <c r="I35" s="10" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J35" s="10" t="b">
+      <c r="I35" s="6" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J35" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3512,11 +3584,11 @@
         <v>1</v>
       </c>
       <c r="H36" s="12"/>
-      <c r="I36" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J36" s="15" t="b">
+      <c r="I36" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3548,11 +3620,11 @@
       </c>
       <c r="G37" s="9"/>
       <c r="H37" s="6"/>
-      <c r="I37" s="10" t="b">
+      <c r="I37" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J37" s="10" t="b">
+      <c r="J37" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3584,11 +3656,11 @@
       </c>
       <c r="G38" s="14"/>
       <c r="H38" s="12"/>
-      <c r="I38" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J38" s="15" t="b">
+      <c r="I38" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J38" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3620,11 +3692,11 @@
       </c>
       <c r="G39" s="9"/>
       <c r="H39" s="6"/>
-      <c r="I39" s="10" t="b">
+      <c r="I39" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J39" s="10" t="b">
+      <c r="J39" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3690,11 +3762,11 @@
       </c>
       <c r="G41" s="9"/>
       <c r="H41" s="6"/>
-      <c r="I41" s="10" t="b">
+      <c r="I41" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J41" s="10" t="b">
+      <c r="J41" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3726,11 +3798,11 @@
       </c>
       <c r="G42" s="14"/>
       <c r="H42" s="12"/>
-      <c r="I42" s="15" t="b">
+      <c r="I42" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J42" s="15" t="b">
+      <c r="J42" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3742,7 +3814,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="33" t="s">
         <v>175</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -3762,11 +3834,11 @@
       </c>
       <c r="G43" s="9"/>
       <c r="H43" s="6"/>
-      <c r="I43" s="10" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J43" s="10" t="b">
+      <c r="I43" s="6" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J43" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3778,7 +3850,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="34" t="s">
         <v>179</v>
       </c>
       <c r="B44" s="12" t="s">
@@ -3798,11 +3870,11 @@
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="15" t="b">
+      <c r="I44" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J44" s="15" t="b">
+      <c r="J44" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3814,7 +3886,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="33" t="s">
         <v>182</v>
       </c>
       <c r="B45" s="6" t="s">
@@ -3834,11 +3906,11 @@
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="6"/>
-      <c r="I45" s="10" t="b">
+      <c r="I45" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J45" s="10" t="b">
+      <c r="J45" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3850,7 +3922,7 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="34" t="s">
         <v>186</v>
       </c>
       <c r="B46" s="12" t="s">
@@ -3870,11 +3942,11 @@
       </c>
       <c r="G46" s="14"/>
       <c r="H46" s="12"/>
-      <c r="I46" s="15" t="b">
+      <c r="I46" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J46" s="15" t="b">
+      <c r="J46" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3906,11 +3978,11 @@
       </c>
       <c r="G47" s="9"/>
       <c r="H47" s="6"/>
-      <c r="I47" s="10" t="b">
+      <c r="I47" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J47" s="10" t="b">
+      <c r="J47" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3922,7 +3994,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="34" t="s">
         <v>194</v>
       </c>
       <c r="B48" s="12" t="s">
@@ -3942,11 +4014,11 @@
       </c>
       <c r="G48" s="14"/>
       <c r="H48" s="12"/>
-      <c r="I48" s="15" t="b">
+      <c r="I48" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J48" s="15" t="b">
+      <c r="J48" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3958,36 +4030,36 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="B49" s="38" t="s">
+      <c r="B49" s="36" t="s">
         <v>199</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C49" s="36" t="s">
         <v>200</v>
       </c>
-      <c r="D49" s="38" t="n">
+      <c r="D49" s="36" t="n">
         <v>4</v>
       </c>
-      <c r="E49" s="39" t="s">
+      <c r="E49" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="F49" s="38" t="s">
+      <c r="F49" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="J49" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="K49" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L49" s="40" t="s">
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J49" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" s="38" t="s">
         <v>85</v>
       </c>
     </row>
@@ -4014,11 +4086,11 @@
         <v>1</v>
       </c>
       <c r="H50" s="12"/>
-      <c r="I50" s="15" t="b">
+      <c r="I50" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J50" s="15" t="b">
+      <c r="J50" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4052,11 +4124,11 @@
         <v>1</v>
       </c>
       <c r="H51" s="18"/>
-      <c r="I51" s="22" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J51" s="22" t="b">
+      <c r="I51" s="18" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J51" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4090,11 +4162,11 @@
         <v>1</v>
       </c>
       <c r="H52" s="12"/>
-      <c r="I52" s="15" t="b">
+      <c r="I52" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J52" s="15" t="b">
+      <c r="J52" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4128,11 +4200,11 @@
         <v>1</v>
       </c>
       <c r="H53" s="18"/>
-      <c r="I53" s="22" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J53" s="22" t="b">
+      <c r="I53" s="18" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J53" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4202,11 +4274,11 @@
         <v>1</v>
       </c>
       <c r="H55" s="12"/>
-      <c r="I55" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J55" s="15" t="b">
+      <c r="I55" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J55" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4227,7 +4299,7 @@
       <c r="C56" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="D56" s="38" t="n">
+      <c r="D56" s="36" t="n">
         <v>60</v>
       </c>
       <c r="E56" s="20" t="s">
@@ -4239,19 +4311,19 @@
       <c r="G56" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="H56" s="38"/>
-      <c r="I56" s="41" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J56" s="41" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K56" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" s="40" t="s">
+      <c r="H56" s="36"/>
+      <c r="I56" s="36" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J56" s="36" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K56" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" s="38" t="s">
         <v>230</v>
       </c>
     </row>
@@ -4276,11 +4348,11 @@
       </c>
       <c r="G57" s="14"/>
       <c r="H57" s="14"/>
-      <c r="I57" s="42" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J57" s="42" t="b">
+      <c r="I57" s="14" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J57" s="14" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4292,7 +4364,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="24.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="43" t="s">
+      <c r="A58" s="39" t="s">
         <v>236</v>
       </c>
       <c r="B58" s="18" t="s">
@@ -4301,7 +4373,7 @@
       <c r="C58" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="D58" s="43" t="n">
+      <c r="D58" s="39" t="n">
         <v>2</v>
       </c>
       <c r="E58" s="20" t="s">
@@ -4312,11 +4384,11 @@
       </c>
       <c r="G58" s="21"/>
       <c r="H58" s="21"/>
-      <c r="I58" s="44" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J58" s="44" t="b">
+      <c r="I58" s="21" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J58" s="21" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4328,7 +4400,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="34" t="s">
         <v>240</v>
       </c>
       <c r="B59" s="12" t="s">
@@ -4348,11 +4420,11 @@
       </c>
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
-      <c r="I59" s="42" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J59" s="42" t="b">
+      <c r="I59" s="14" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J59" s="14" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4364,7 +4436,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="33" t="s">
         <v>243</v>
       </c>
       <c r="B60" s="6" t="s">
@@ -4384,11 +4456,11 @@
       </c>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
-      <c r="I60" s="45" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J60" s="45" t="b">
+      <c r="I60" s="9" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J60" s="9" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4420,11 +4492,11 @@
       </c>
       <c r="G61" s="14"/>
       <c r="H61" s="12"/>
-      <c r="I61" s="15" t="b">
+      <c r="I61" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J61" s="15" t="b">
+      <c r="J61" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4445,7 +4517,7 @@
       <c r="C62" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="D62" s="43" t="n">
+      <c r="D62" s="39" t="n">
         <v>12</v>
       </c>
       <c r="E62" s="20" t="s">
@@ -4456,11 +4528,11 @@
       </c>
       <c r="G62" s="21"/>
       <c r="H62" s="18"/>
-      <c r="I62" s="22" t="b">
+      <c r="I62" s="18" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J62" s="22" t="b">
+      <c r="J62" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4484,7 +4556,7 @@
       <c r="D63" s="18" t="n">
         <v>4</v>
       </c>
-      <c r="E63" s="46" t="s">
+      <c r="E63" s="40" t="s">
         <v>257</v>
       </c>
       <c r="F63" s="18" t="s">
@@ -4492,11 +4564,11 @@
       </c>
       <c r="G63" s="21"/>
       <c r="H63" s="18"/>
-      <c r="I63" s="22" t="b">
+      <c r="I63" s="18" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J63" s="22" t="b">
+      <c r="J63" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4528,11 +4600,11 @@
       </c>
       <c r="G64" s="14"/>
       <c r="H64" s="12"/>
-      <c r="I64" s="15" t="b">
+      <c r="I64" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J64" s="15" t="b">
+      <c r="J64" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4544,7 +4616,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="43" t="s">
+      <c r="A65" s="39" t="s">
         <v>263</v>
       </c>
       <c r="B65" s="18" t="s">
@@ -4553,7 +4625,7 @@
       <c r="C65" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="D65" s="43" t="n">
+      <c r="D65" s="39" t="n">
         <v>4</v>
       </c>
       <c r="E65" s="20" t="s">
@@ -4564,11 +4636,11 @@
       </c>
       <c r="G65" s="21"/>
       <c r="H65" s="18"/>
-      <c r="I65" s="22" t="b">
+      <c r="I65" s="18" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J65" s="22" t="b">
+      <c r="J65" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4600,11 +4672,11 @@
       </c>
       <c r="G66" s="14"/>
       <c r="H66" s="12"/>
-      <c r="I66" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J66" s="15" t="b">
+      <c r="I66" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J66" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4616,7 +4688,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="43" t="s">
+      <c r="A67" s="39" t="s">
         <v>272</v>
       </c>
       <c r="B67" s="18" t="s">
@@ -4625,7 +4697,7 @@
       <c r="C67" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="D67" s="43" t="n">
+      <c r="D67" s="39" t="n">
         <v>8</v>
       </c>
       <c r="E67" s="20" t="s">
@@ -4640,7 +4712,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J67" s="22" t="b">
+      <c r="J67" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4700,7 +4772,7 @@
       <c r="D69" s="31" t="n">
         <v>4</v>
       </c>
-      <c r="E69" s="47" t="s">
+      <c r="E69" s="41" t="s">
         <v>284</v>
       </c>
       <c r="F69" s="18" t="s">
@@ -4712,7 +4784,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J69" s="22" t="b">
+      <c r="J69" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4746,11 +4818,11 @@
         <v>4</v>
       </c>
       <c r="H70" s="12"/>
-      <c r="I70" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J70" s="15" t="b">
+      <c r="I70" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J70" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4784,11 +4856,11 @@
         <v>4</v>
       </c>
       <c r="H71" s="18"/>
-      <c r="I71" s="22" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J71" s="22" t="b">
+      <c r="I71" s="18" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J71" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4822,11 +4894,11 @@
         <v>3</v>
       </c>
       <c r="H72" s="12"/>
-      <c r="I72" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J72" s="15" t="b">
+      <c r="I72" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J72" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4850,7 +4922,7 @@
       <c r="D73" s="18" t="n">
         <v>48</v>
       </c>
-      <c r="E73" s="48"/>
+      <c r="E73" s="42"/>
       <c r="F73" s="18" t="s">
         <v>64</v>
       </c>
@@ -4858,11 +4930,11 @@
         <v>3</v>
       </c>
       <c r="H73" s="6"/>
-      <c r="I73" s="10" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J73" s="10" t="b">
+      <c r="I73" s="6" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J73" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4894,11 +4966,11 @@
         <v>5</v>
       </c>
       <c r="H74" s="12"/>
-      <c r="I74" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J74" s="15" t="b">
+      <c r="I74" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J74" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4910,7 +4982,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="49" t="s">
+      <c r="A75" s="43" t="s">
         <v>307</v>
       </c>
       <c r="B75" s="7" t="s">
@@ -4934,7 +5006,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J75" s="10" t="b">
+      <c r="J75" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4966,11 +5038,11 @@
       </c>
       <c r="G76" s="14"/>
       <c r="H76" s="12"/>
-      <c r="I76" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J76" s="15" t="b">
+      <c r="I76" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J76" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4982,7 +5054,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="50" t="s">
+      <c r="A77" s="44" t="s">
         <v>316</v>
       </c>
       <c r="B77" s="21" t="s">
@@ -4991,10 +5063,10 @@
       <c r="C77" s="21" t="s">
         <v>318</v>
       </c>
-      <c r="D77" s="43" t="n">
+      <c r="D77" s="39" t="n">
         <v>12</v>
       </c>
-      <c r="E77" s="51" t="s">
+      <c r="E77" s="45" t="s">
         <v>319</v>
       </c>
       <c r="F77" s="18" t="s">
@@ -5004,11 +5076,11 @@
         <v>-1</v>
       </c>
       <c r="H77" s="18"/>
-      <c r="I77" s="22" t="b">
+      <c r="I77" s="18" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J77" s="22" t="b">
+      <c r="J77" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5020,7 +5092,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="36" t="s">
+      <c r="A78" s="34" t="s">
         <v>321</v>
       </c>
       <c r="B78" s="12" t="s">
@@ -5040,11 +5112,11 @@
         <v>5</v>
       </c>
       <c r="H78" s="12"/>
-      <c r="I78" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J78" s="15" t="b">
+      <c r="I78" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J78" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5076,11 +5148,11 @@
         <v>2</v>
       </c>
       <c r="H79" s="6"/>
-      <c r="I79" s="10" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J79" s="10" t="b">
+      <c r="I79" s="6" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J79" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5112,11 +5184,11 @@
       </c>
       <c r="G80" s="14"/>
       <c r="H80" s="12"/>
-      <c r="I80" s="15" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J80" s="15" t="b">
+      <c r="I80" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J80" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5148,11 +5220,11 @@
       </c>
       <c r="G81" s="21"/>
       <c r="H81" s="6"/>
-      <c r="I81" s="10" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J81" s="10" t="b">
+      <c r="I81" s="6" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J81" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5184,11 +5256,11 @@
       </c>
       <c r="G82" s="14"/>
       <c r="H82" s="12"/>
-      <c r="I82" s="15" t="b">
+      <c r="I82" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J82" s="15" t="b">
+      <c r="J82" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5200,66 +5272,66 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="38" t="s">
+      <c r="A83" s="36" t="s">
         <v>339</v>
       </c>
-      <c r="B83" s="38" t="s">
+      <c r="B83" s="36" t="s">
         <v>340</v>
       </c>
-      <c r="C83" s="38" t="s">
+      <c r="C83" s="36" t="s">
         <v>341</v>
       </c>
-      <c r="D83" s="38" t="n">
+      <c r="D83" s="36" t="n">
         <v>8</v>
       </c>
-      <c r="E83" s="52" t="s">
+      <c r="E83" s="46" t="s">
         <v>342</v>
       </c>
-      <c r="F83" s="38" t="s">
+      <c r="F83" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="G83" s="38" t="n">
+      <c r="G83" s="36" t="n">
         <v>5</v>
       </c>
-      <c r="H83" s="53"/>
-      <c r="I83" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J83" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="K83" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="L83" s="40" t="s">
+      <c r="H83" s="47"/>
+      <c r="I83" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K83" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L83" s="38" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="38" t="s">
+      <c r="A84" s="36" t="s">
         <v>344</v>
       </c>
-      <c r="B84" s="40" t="s">
+      <c r="B84" s="38" t="s">
         <v>345</v>
       </c>
-      <c r="C84" s="38" t="s">
+      <c r="C84" s="36" t="s">
         <v>346</v>
       </c>
-      <c r="D84" s="38" t="n">
+      <c r="D84" s="36" t="n">
         <v>8</v>
       </c>
-      <c r="E84" s="52" t="s">
+      <c r="E84" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="F84" s="54" t="s">
+      <c r="F84" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G84" s="38"/>
-      <c r="H84" s="53"/>
-      <c r="I84" s="53"/>
-      <c r="J84" s="53"/>
-      <c r="K84" s="53"/>
-      <c r="L84" s="38" t="s">
+      <c r="G84" s="36"/>
+      <c r="H84" s="47"/>
+      <c r="I84" s="47"/>
+      <c r="J84" s="47"/>
+      <c r="K84" s="47"/>
+      <c r="L84" s="36" t="s">
         <v>348</v>
       </c>
     </row>
@@ -5284,11 +5356,11 @@
       </c>
       <c r="G85" s="14"/>
       <c r="H85" s="12"/>
-      <c r="I85" s="15" t="b">
+      <c r="I85" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J85" s="15" t="b">
+      <c r="J85" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5320,11 +5392,11 @@
       </c>
       <c r="G86" s="21"/>
       <c r="H86" s="18"/>
-      <c r="I86" s="22" t="b">
+      <c r="I86" s="18" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J86" s="22" t="b">
+      <c r="J86" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5356,11 +5428,11 @@
       </c>
       <c r="G87" s="14"/>
       <c r="H87" s="12"/>
-      <c r="I87" s="15" t="b">
+      <c r="I87" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J87" s="15" t="b">
+      <c r="J87" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5392,11 +5464,11 @@
       </c>
       <c r="G88" s="9"/>
       <c r="H88" s="6"/>
-      <c r="I88" s="10" t="b">
+      <c r="I88" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J88" s="10" t="b">
+      <c r="J88" s="6" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5428,11 +5500,11 @@
       </c>
       <c r="G89" s="14"/>
       <c r="H89" s="12"/>
-      <c r="I89" s="15" t="b">
+      <c r="I89" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J89" s="15" t="b">
+      <c r="J89" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5476,7 +5548,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="43" t="s">
+      <c r="A91" s="39" t="s">
         <v>371</v>
       </c>
       <c r="B91" s="18" t="s">
@@ -5485,7 +5557,7 @@
       <c r="C91" s="18" t="s">
         <v>373</v>
       </c>
-      <c r="D91" s="43" t="n">
+      <c r="D91" s="39" t="n">
         <v>4</v>
       </c>
       <c r="E91" s="20" t="s">
@@ -5500,7 +5572,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J91" s="22" t="b">
+      <c r="J91" s="18" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5546,7 +5618,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="36" t="s">
+      <c r="A93" s="34" t="s">
         <v>381</v>
       </c>
       <c r="B93" s="12" t="s">
@@ -5620,7 +5692,7 @@
       <c r="B95" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="C95" s="33" t="s">
+      <c r="C95" s="12" t="s">
         <v>391</v>
       </c>
       <c r="D95" s="12" t="n">
@@ -5750,36 +5822,36 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="38" t="s">
+      <c r="A99" s="36" t="s">
         <v>404</v>
       </c>
-      <c r="B99" s="38" t="s">
+      <c r="B99" s="36" t="s">
         <v>405</v>
       </c>
-      <c r="C99" s="38" t="s">
+      <c r="C99" s="36" t="s">
         <v>406</v>
       </c>
-      <c r="D99" s="38" t="n">
+      <c r="D99" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="E99" s="39" t="s">
+      <c r="E99" s="37" t="s">
         <v>407</v>
       </c>
-      <c r="F99" s="38" t="s">
+      <c r="F99" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="G99" s="38"/>
-      <c r="H99" s="53"/>
-      <c r="I99" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="J99" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="K99" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="L99" s="40" t="s">
+      <c r="G99" s="36"/>
+      <c r="H99" s="47"/>
+      <c r="I99" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="J99" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L99" s="38" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6006,7 +6078,7 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="43" t="s">
+      <c r="A107" s="39" t="s">
         <v>437</v>
       </c>
       <c r="B107" s="18" t="s">
@@ -6015,7 +6087,7 @@
       <c r="C107" s="18" t="s">
         <v>439</v>
       </c>
-      <c r="D107" s="43" t="n">
+      <c r="D107" s="39" t="n">
         <v>8</v>
       </c>
       <c r="E107" s="20" t="s">
@@ -6039,68 +6111,13 @@
         <v>441</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="55"/>
-      <c r="B110" s="55"/>
-      <c r="C110" s="56" t="s">
-        <v>442</v>
-      </c>
-      <c r="D110" s="55"/>
-      <c r="E110" s="57"/>
-      <c r="F110" s="58"/>
-      <c r="G110" s="58"/>
-      <c r="H110" s="0"/>
-      <c r="I110" s="0"/>
-      <c r="J110" s="0"/>
-      <c r="K110" s="0"/>
-      <c r="L110" s="0"/>
-    </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="55"/>
-      <c r="B111" s="55"/>
-      <c r="C111" s="56"/>
-      <c r="D111" s="55"/>
-      <c r="E111" s="57"/>
-      <c r="F111" s="58"/>
-      <c r="G111" s="58"/>
-      <c r="H111" s="0"/>
-      <c r="I111" s="0"/>
-      <c r="J111" s="0"/>
-      <c r="K111" s="0"/>
-      <c r="L111" s="0"/>
-    </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="59" t="s">
-        <v>443</v>
-      </c>
-      <c r="B112" s="60" t="s">
-        <v>444</v>
-      </c>
-      <c r="C112" s="61"/>
-      <c r="D112" s="55"/>
-      <c r="E112" s="57"/>
-      <c r="F112" s="58"/>
-      <c r="G112" s="58"/>
-      <c r="H112" s="0"/>
-      <c r="I112" s="0"/>
-      <c r="J112" s="0"/>
-      <c r="K112" s="0"/>
-      <c r="L112" s="0"/>
-    </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="62"/>
-      <c r="B113" s="63" t="s">
-        <v>445</v>
-      </c>
-      <c r="C113" s="64"/>
-    </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="65"/>
-      <c r="B114" s="66" t="s">
-        <v>446</v>
-      </c>
-      <c r="C114" s="67"/>
-    </row>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6147,7 +6164,7 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.451388888888889" right="0.634027777777778" top="0.513194444444444" bottom="0.338194444444444" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.451388888888889" right="0.634027777777778" top="0.513194444444445" bottom="0.338194444444444" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="65" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -6157,18 +6174,141 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="49" t="s">
+        <v>442</v>
+      </c>
+      <c r="D3" s="48"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="52" t="s">
+        <v>443</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>444</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="55"/>
+      <c r="B6" s="56" t="s">
+        <v>445</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="58"/>
+      <c r="B7" s="59" t="s">
+        <v>446</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
made external classroom exclusive if alternating week is True
</commit_message>
<xml_diff>
--- a/db_info/projeto2024.xlsx
+++ b/db_info/projeto2024.xlsx
@@ -1611,7 +1611,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1660,6 +1660,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1704,7 +1708,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1729,37 +1733,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF7F7F7"/>
-          <bgColor rgb="FF272727"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF9900FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1831,23 +1804,19 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.4765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="63.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="62.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="31.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="62.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="1" width="16.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="68.05"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="3" width="12.49"/>
@@ -1916,7 +1885,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J2" s="11" t="b">
+      <c r="J2" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1928,7 +1897,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1937,7 +1906,7 @@
       <c r="C3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="13" t="n">
+      <c r="D3" s="14" t="n">
         <v>2</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -1961,7 +1930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
@@ -1995,7 +1964,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
@@ -2022,7 +1991,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J5" s="11" t="b">
+      <c r="J5" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2033,7 +2002,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
@@ -2060,7 +2029,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J6" s="11" t="b">
+      <c r="J6" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2071,7 +2040,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>39</v>
       </c>
@@ -2096,7 +2065,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J7" s="11" t="b">
+      <c r="J7" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2120,7 +2089,7 @@
       <c r="D8" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="16" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -2134,7 +2103,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J8" s="11" t="b">
+      <c r="J8" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2164,11 +2133,11 @@
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="11" t="b">
+      <c r="I9" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J9" s="11" t="b">
+      <c r="J9" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2202,22 +2171,22 @@
       <c r="H10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="11" t="b">
+      <c r="I10" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J10" s="11" t="b">
+      <c r="J10" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K10" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>55</v>
       </c>
@@ -2238,11 +2207,11 @@
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="11" t="b">
+      <c r="I11" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J11" s="11" t="b">
+      <c r="J11" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2253,8 +2222,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+    <row r="12" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="s">
         <v>59</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2263,7 +2232,7 @@
       <c r="C12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="13" t="n">
+      <c r="D12" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E12" s="9" t="s">
@@ -2276,11 +2245,11 @@
       <c r="H12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="11" t="b">
+      <c r="I12" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J12" s="11" t="b">
+      <c r="J12" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2314,11 +2283,11 @@
         <v>1</v>
       </c>
       <c r="H13" s="7"/>
-      <c r="I13" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J13" s="11" t="b">
+      <c r="I13" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2329,8 +2298,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
+    <row r="14" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
         <v>69</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2339,7 +2308,7 @@
       <c r="C14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="13" t="n">
+      <c r="D14" s="14" t="n">
         <v>8</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -2352,22 +2321,22 @@
       <c r="H14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="11" t="b">
+      <c r="I14" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J14" s="11" t="b">
+      <c r="J14" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K14" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>73</v>
       </c>
@@ -2390,11 +2359,11 @@
         <v>1</v>
       </c>
       <c r="H15" s="7"/>
-      <c r="I15" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="11" t="b">
+      <c r="I15" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2405,7 +2374,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
         <v>77</v>
       </c>
@@ -2433,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>46</v>
@@ -2502,7 +2471,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J18" s="11" t="b">
+      <c r="J18" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2538,7 +2507,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J19" s="11" t="b">
+      <c r="J19" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2576,7 +2545,7 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="J20" s="11" t="b">
+      <c r="J20" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2608,11 +2577,11 @@
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="11" t="b">
+      <c r="I21" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J21" s="11" t="b">
+      <c r="J21" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2646,11 +2615,11 @@
       <c r="H22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="11" t="b">
+      <c r="I22" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J22" s="11" t="b">
+      <c r="J22" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2684,11 +2653,11 @@
         <v>1</v>
       </c>
       <c r="H23" s="7"/>
-      <c r="I23" s="11" t="b">
+      <c r="I23" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J23" s="11" t="b">
+      <c r="J23" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2725,7 +2694,7 @@
       <c r="I24" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J24" s="11" t="b">
+      <c r="J24" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2757,11 +2726,11 @@
         <v>1</v>
       </c>
       <c r="H25" s="7"/>
-      <c r="I25" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J25" s="11" t="b">
+      <c r="I25" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2795,11 +2764,11 @@
         <v>1</v>
       </c>
       <c r="H26" s="7"/>
-      <c r="I26" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="11" t="b">
+      <c r="I26" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2831,11 +2800,11 @@
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="11" t="b">
+      <c r="I27" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J27" s="11" t="b">
+      <c r="J27" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2867,11 +2836,11 @@
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="7"/>
-      <c r="I28" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J28" s="11" t="b">
+      <c r="I28" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2892,7 +2861,7 @@
       <c r="C29" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="16" t="n">
+      <c r="D29" s="17" t="n">
         <v>2</v>
       </c>
       <c r="E29" s="9" t="s">
@@ -2905,11 +2874,11 @@
       <c r="H29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="11" t="b">
+      <c r="I29" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J29" s="11" t="b">
+      <c r="J29" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2920,7 +2889,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
         <v>134</v>
       </c>
@@ -2943,11 +2912,11 @@
       <c r="H30" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="11" t="b">
+      <c r="I30" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J30" s="11" t="b">
+      <c r="J30" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2958,7 +2927,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
         <v>138</v>
       </c>
@@ -2981,11 +2950,11 @@
       <c r="H31" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="11" t="b">
+      <c r="I31" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J31" s="11" t="b">
+      <c r="J31" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2996,7 +2965,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
         <v>140</v>
       </c>
@@ -3019,11 +2988,11 @@
       <c r="H32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="11" t="b">
+      <c r="I32" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J32" s="11" t="b">
+      <c r="J32" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3034,7 +3003,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
         <v>144</v>
       </c>
@@ -3057,11 +3026,11 @@
       <c r="H33" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I33" s="11" t="b">
+      <c r="I33" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J33" s="11" t="b">
+      <c r="J33" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3095,11 +3064,11 @@
       <c r="H34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="11" t="b">
+      <c r="I34" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J34" s="11" t="b">
+      <c r="J34" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3133,11 +3102,11 @@
       <c r="H35" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I35" s="11" t="b">
+      <c r="I35" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J35" s="11" t="b">
+      <c r="J35" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3171,11 +3140,11 @@
       <c r="H36" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I36" s="11" t="b">
+      <c r="I36" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J36" s="11" t="b">
+      <c r="J36" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3209,11 +3178,11 @@
       <c r="H37" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I37" s="11" t="b">
+      <c r="I37" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J37" s="11" t="b">
+      <c r="J37" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3225,7 +3194,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="18" t="s">
         <v>158</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -3237,7 +3206,7 @@
       <c r="D38" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E38" s="18"/>
+      <c r="E38" s="19"/>
       <c r="F38" s="7" t="s">
         <v>16</v>
       </c>
@@ -3245,11 +3214,11 @@
       <c r="H38" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I38" s="11" t="b">
+      <c r="I38" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J38" s="11" t="b">
+      <c r="J38" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3279,15 +3248,15 @@
       <c r="F39" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="19"/>
+      <c r="G39" s="20"/>
       <c r="H39" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="11" t="b">
+      <c r="I39" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J39" s="11" t="b">
+      <c r="J39" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3308,24 +3277,24 @@
       <c r="C40" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="D40" s="16" t="n">
+      <c r="D40" s="17" t="n">
         <v>2</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G40" s="21"/>
+      <c r="G40" s="22"/>
       <c r="H40" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I40" s="11" t="b">
+      <c r="I40" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J40" s="11" t="b">
+      <c r="J40" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3337,7 +3306,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="14" t="s">
         <v>167</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -3346,7 +3315,7 @@
       <c r="C41" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D41" s="13" t="n">
+      <c r="D41" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E41" s="9" t="s">
@@ -3357,23 +3326,23 @@
       </c>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
-      <c r="I41" s="11" t="b">
+      <c r="I41" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J41" s="11" t="b">
+      <c r="J41" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K41" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" s="7" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="13" t="s">
         <v>172</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -3382,7 +3351,7 @@
       <c r="C42" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D42" s="13" t="n">
+      <c r="D42" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E42" s="9" t="s">
@@ -3393,23 +3362,23 @@
       </c>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
-      <c r="I42" s="11" t="b">
+      <c r="I42" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J42" s="11" t="b">
+      <c r="J42" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K42" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" s="7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="23" t="s">
         <v>177</v>
       </c>
       <c r="B43" s="10" t="s">
@@ -3421,7 +3390,7 @@
       <c r="D43" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="19" t="s">
         <v>180</v>
       </c>
       <c r="F43" s="10" t="s">
@@ -3436,14 +3405,14 @@
         <v>0</v>
       </c>
       <c r="K43" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L43" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="14" t="s">
         <v>181</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -3452,7 +3421,7 @@
       <c r="C44" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D44" s="13" t="n">
+      <c r="D44" s="14" t="n">
         <v>8</v>
       </c>
       <c r="E44" s="9" t="s">
@@ -3470,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44" s="10" t="s">
         <v>171</v>
@@ -3497,16 +3466,16 @@
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
-      <c r="I45" s="11" t="b">
+      <c r="I45" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J45" s="11" t="b">
+      <c r="J45" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K45" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L45" s="7" t="s">
         <v>171</v>
@@ -3533,23 +3502,23 @@
       </c>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
-      <c r="I46" s="11" t="b">
+      <c r="I46" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J46" s="11" t="b">
+      <c r="J46" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K46" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" s="7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="13" t="s">
         <v>191</v>
       </c>
       <c r="B47" s="7" t="s">
@@ -3558,7 +3527,7 @@
       <c r="C47" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D47" s="13" t="n">
+      <c r="D47" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E47" s="9" t="s">
@@ -3569,23 +3538,23 @@
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
-      <c r="I47" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J47" s="11" t="b">
+      <c r="I47" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K47" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L47" s="7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B48" s="7" t="s">
@@ -3594,7 +3563,7 @@
       <c r="C48" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D48" s="13" t="n">
+      <c r="D48" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E48" s="9" t="s">
@@ -3605,23 +3574,23 @@
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
-      <c r="I48" s="11" t="b">
+      <c r="I48" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J48" s="11" t="b">
+      <c r="J48" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K48" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48" s="7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="13" t="s">
         <v>198</v>
       </c>
       <c r="B49" s="7" t="s">
@@ -3630,7 +3599,7 @@
       <c r="C49" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="D49" s="13" t="n">
+      <c r="D49" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E49" s="9" t="s">
@@ -3641,23 +3610,23 @@
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
-      <c r="I49" s="11" t="b">
+      <c r="I49" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J49" s="11" t="b">
+      <c r="J49" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K49" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L49" s="7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="13" t="s">
         <v>202</v>
       </c>
       <c r="B50" s="7" t="s">
@@ -3666,7 +3635,7 @@
       <c r="C50" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D50" s="13" t="n">
+      <c r="D50" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E50" s="9" t="s">
@@ -3677,16 +3646,16 @@
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="7"/>
-      <c r="I50" s="11" t="b">
+      <c r="I50" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J50" s="11" t="b">
+      <c r="J50" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K50" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L50" s="7" t="s">
         <v>176</v>
@@ -3713,16 +3682,16 @@
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
-      <c r="I51" s="11" t="b">
+      <c r="I51" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J51" s="11" t="b">
+      <c r="J51" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K51" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" s="7" t="s">
         <v>176</v>
@@ -3751,11 +3720,11 @@
         <v>1</v>
       </c>
       <c r="H52" s="7"/>
-      <c r="I52" s="11" t="b">
+      <c r="I52" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J52" s="11" t="b">
+      <c r="J52" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3767,7 +3736,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="13" t="s">
         <v>215</v>
       </c>
       <c r="B53" s="7" t="s">
@@ -3776,7 +3745,7 @@
       <c r="C53" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D53" s="13" t="n">
+      <c r="D53" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E53" s="9" t="s">
@@ -3787,11 +3756,11 @@
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
-      <c r="I53" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J53" s="11" t="b">
+      <c r="I53" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J53" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3825,11 +3794,11 @@
         <v>1</v>
       </c>
       <c r="H54" s="7"/>
-      <c r="I54" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J54" s="11" t="b">
+      <c r="I54" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J54" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3863,11 +3832,11 @@
         <v>1</v>
       </c>
       <c r="H55" s="7"/>
-      <c r="I55" s="11" t="b">
+      <c r="I55" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J55" s="11" t="b">
+      <c r="J55" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3901,11 +3870,11 @@
         <v>1</v>
       </c>
       <c r="H56" s="7"/>
-      <c r="I56" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J56" s="11" t="b">
+      <c r="I56" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J56" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3975,11 +3944,11 @@
         <v>1</v>
       </c>
       <c r="H58" s="7"/>
-      <c r="I58" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J58" s="11" t="b">
+      <c r="I58" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J58" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4013,11 +3982,11 @@
         <v>1</v>
       </c>
       <c r="H59" s="7"/>
-      <c r="I59" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J59" s="11" t="b">
+      <c r="I59" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J59" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4049,11 +4018,11 @@
       </c>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
-      <c r="I60" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J60" s="11" t="b">
+      <c r="I60" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J60" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4065,7 +4034,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="14" t="s">
         <v>249</v>
       </c>
       <c r="B61" s="7" t="s">
@@ -4074,7 +4043,7 @@
       <c r="C61" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="D61" s="13" t="n">
+      <c r="D61" s="14" t="n">
         <v>2</v>
       </c>
       <c r="E61" s="9" t="s">
@@ -4085,11 +4054,11 @@
       </c>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
-      <c r="I61" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J61" s="11" t="b">
+      <c r="I61" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J61" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4101,7 +4070,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="13" t="s">
         <v>253</v>
       </c>
       <c r="B62" s="7" t="s">
@@ -4110,7 +4079,7 @@
       <c r="C62" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D62" s="13" t="n">
+      <c r="D62" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E62" s="9" t="s">
@@ -4121,11 +4090,11 @@
       </c>
       <c r="G62" s="10"/>
       <c r="H62" s="10"/>
-      <c r="I62" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J62" s="23" t="b">
+      <c r="I62" s="24" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J62" s="24" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4171,7 +4140,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="13" t="s">
+      <c r="A64" s="14" t="s">
         <v>261</v>
       </c>
       <c r="B64" s="7" t="s">
@@ -4180,7 +4149,7 @@
       <c r="C64" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="D64" s="13" t="n">
+      <c r="D64" s="14" t="n">
         <v>8</v>
       </c>
       <c r="E64" s="9" t="s">
@@ -4191,16 +4160,16 @@
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
-      <c r="I64" s="11" t="b">
+      <c r="I64" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J64" s="11" t="b">
+      <c r="J64" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K64" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L64" s="7" t="s">
         <v>176</v>
@@ -4219,21 +4188,21 @@
       <c r="D65" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E65" s="18" t="s">
+      <c r="E65" s="19" t="s">
         <v>268</v>
       </c>
       <c r="F65" s="10" t="s">
         <v>27</v>
       </c>
       <c r="G65" s="10"/>
-      <c r="H65" s="24"/>
-      <c r="I65" s="24" t="n">
-        <v>1</v>
-      </c>
-      <c r="J65" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="K65" s="24" t="n">
+      <c r="H65" s="25"/>
+      <c r="I65" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J65" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" s="25" t="n">
         <v>1</v>
       </c>
       <c r="L65" s="7" t="s">
@@ -4275,7 +4244,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="14" t="s">
         <v>273</v>
       </c>
       <c r="B67" s="7" t="s">
@@ -4311,7 +4280,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="13" t="s">
+      <c r="A68" s="14" t="s">
         <v>278</v>
       </c>
       <c r="B68" s="7" t="s">
@@ -4320,7 +4289,7 @@
       <c r="C68" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="D68" s="13" t="n">
+      <c r="D68" s="14" t="n">
         <v>2</v>
       </c>
       <c r="E68" s="9" t="s">
@@ -4344,7 +4313,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="69" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="7" t="s">
         <v>282</v>
       </c>
@@ -4365,22 +4334,22 @@
       </c>
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
-      <c r="I69" s="11" t="b">
+      <c r="I69" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J69" s="11" t="b">
+      <c r="J69" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K69" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L69" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="70" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="7" t="s">
         <v>285</v>
       </c>
@@ -4390,7 +4359,7 @@
       <c r="C70" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="D70" s="13" t="n">
+      <c r="D70" s="14" t="n">
         <v>12</v>
       </c>
       <c r="E70" s="9" t="s">
@@ -4401,11 +4370,11 @@
       </c>
       <c r="G70" s="10"/>
       <c r="H70" s="7"/>
-      <c r="I70" s="11" t="b">
+      <c r="I70" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J70" s="11" t="b">
+      <c r="J70" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4416,7 +4385,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="71" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="7" t="s">
         <v>289</v>
       </c>
@@ -4450,7 +4419,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="72" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="7" t="s">
         <v>293</v>
       </c>
@@ -4463,7 +4432,7 @@
       <c r="D72" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="E72" s="25" t="s">
+      <c r="E72" s="26" t="s">
         <v>296</v>
       </c>
       <c r="F72" s="7" t="s">
@@ -4471,22 +4440,22 @@
       </c>
       <c r="G72" s="10"/>
       <c r="H72" s="7"/>
-      <c r="I72" s="11" t="b">
+      <c r="I72" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J72" s="11" t="b">
+      <c r="J72" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K72" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L72" s="7" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="73" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="8" t="s">
         <v>297</v>
       </c>
@@ -4507,23 +4476,23 @@
       </c>
       <c r="G73" s="10"/>
       <c r="H73" s="7"/>
-      <c r="I73" s="11" t="b">
+      <c r="I73" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J73" s="11" t="b">
+      <c r="J73" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K73" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L73" s="10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="74" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="13" t="s">
+    <row r="74" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="14" t="s">
         <v>300</v>
       </c>
       <c r="B74" s="7" t="s">
@@ -4532,7 +4501,7 @@
       <c r="C74" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="D74" s="13" t="n">
+      <c r="D74" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E74" s="9" t="s">
@@ -4543,11 +4512,11 @@
       </c>
       <c r="G74" s="10"/>
       <c r="H74" s="7"/>
-      <c r="I74" s="11" t="b">
+      <c r="I74" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J74" s="11" t="b">
+      <c r="J74" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4579,16 +4548,16 @@
       </c>
       <c r="G75" s="10"/>
       <c r="H75" s="7"/>
-      <c r="I75" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J75" s="11" t="b">
+      <c r="I75" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J75" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K75" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L75" s="10" t="s">
         <v>176</v>
@@ -4604,10 +4573,10 @@
       <c r="C76" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="D76" s="13" t="n">
+      <c r="D76" s="14" t="n">
         <v>4</v>
       </c>
-      <c r="E76" s="26" t="s">
+      <c r="E76" s="27" t="s">
         <v>312</v>
       </c>
       <c r="F76" s="7" t="s">
@@ -4615,23 +4584,23 @@
       </c>
       <c r="G76" s="10"/>
       <c r="H76" s="7"/>
-      <c r="I76" s="11" t="b">
+      <c r="I76" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J76" s="11" t="b">
+      <c r="J76" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K76" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L76" s="7" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="77" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="12" t="s">
+    <row r="77" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="13" t="s">
         <v>313</v>
       </c>
       <c r="B77" s="7" t="s">
@@ -4640,7 +4609,7 @@
       <c r="C77" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="D77" s="13" t="n">
+      <c r="D77" s="14" t="n">
         <v>40</v>
       </c>
       <c r="E77" s="9"/>
@@ -4651,11 +4620,11 @@
         <v>5</v>
       </c>
       <c r="H77" s="7"/>
-      <c r="I77" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J77" s="11" t="b">
+      <c r="I77" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J77" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4666,7 +4635,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="78" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
         <v>317</v>
       </c>
@@ -4687,11 +4656,11 @@
         <v>2</v>
       </c>
       <c r="H78" s="7"/>
-      <c r="I78" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J78" s="11" t="b">
+      <c r="I78" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J78" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4702,7 +4671,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="79" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
         <v>321</v>
       </c>
@@ -4723,11 +4692,11 @@
       </c>
       <c r="G79" s="10"/>
       <c r="H79" s="7"/>
-      <c r="I79" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J79" s="11" t="b">
+      <c r="I79" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J79" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4759,23 +4728,23 @@
       </c>
       <c r="G80" s="10"/>
       <c r="H80" s="7"/>
-      <c r="I80" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J80" s="11" t="b">
+      <c r="I80" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J80" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K80" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L80" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="13" t="s">
+      <c r="A81" s="14" t="s">
         <v>329</v>
       </c>
       <c r="B81" s="7" t="s">
@@ -4784,7 +4753,7 @@
       <c r="C81" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="D81" s="13" t="n">
+      <c r="D81" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E81" s="9" t="s">
@@ -4795,16 +4764,16 @@
       </c>
       <c r="G81" s="10"/>
       <c r="H81" s="7"/>
-      <c r="I81" s="11" t="b">
+      <c r="I81" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J81" s="11" t="b">
+      <c r="J81" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K81" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L81" s="7" t="s">
         <v>22</v>
@@ -4832,14 +4801,14 @@
       <c r="G82" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="H82" s="24"/>
-      <c r="I82" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="J82" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="K82" s="24" t="n">
+      <c r="H82" s="25"/>
+      <c r="I82" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K82" s="25" t="n">
         <v>0</v>
       </c>
       <c r="L82" s="7" t="s">
@@ -4866,15 +4835,15 @@
         <v>27</v>
       </c>
       <c r="G83" s="10"/>
-      <c r="H83" s="24"/>
-      <c r="I83" s="24"/>
-      <c r="J83" s="24"/>
-      <c r="K83" s="24"/>
+      <c r="H83" s="25"/>
+      <c r="I83" s="25"/>
+      <c r="J83" s="25"/>
+      <c r="K83" s="25"/>
       <c r="L83" s="10" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="84" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
         <v>343</v>
       </c>
@@ -4884,7 +4853,7 @@
       <c r="C84" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="D84" s="13" t="n">
+      <c r="D84" s="14" t="n">
         <v>8</v>
       </c>
       <c r="E84" s="9" t="s">
@@ -4897,11 +4866,11 @@
         <v>4</v>
       </c>
       <c r="H84" s="7"/>
-      <c r="I84" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J84" s="11" t="b">
+      <c r="I84" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J84" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4935,11 +4904,11 @@
         <v>4</v>
       </c>
       <c r="H85" s="7"/>
-      <c r="I85" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J85" s="11" t="b">
+      <c r="I85" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J85" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -4973,11 +4942,11 @@
         <v>3</v>
       </c>
       <c r="H86" s="7"/>
-      <c r="I86" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J86" s="11" t="b">
+      <c r="I86" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J86" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5001,7 +4970,7 @@
       <c r="D87" s="7" t="n">
         <v>48</v>
       </c>
-      <c r="E87" s="18"/>
+      <c r="E87" s="19"/>
       <c r="F87" s="7" t="s">
         <v>27</v>
       </c>
@@ -5009,11 +4978,11 @@
         <v>3</v>
       </c>
       <c r="H87" s="7"/>
-      <c r="I87" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J87" s="11" t="b">
+      <c r="I87" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J87" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5037,7 +5006,7 @@
       <c r="D88" s="7" t="n">
         <v>80</v>
       </c>
-      <c r="E88" s="18"/>
+      <c r="E88" s="19"/>
       <c r="F88" s="7" t="s">
         <v>27</v>
       </c>
@@ -5045,11 +5014,11 @@
         <v>5</v>
       </c>
       <c r="H88" s="7"/>
-      <c r="I88" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J88" s="11" t="b">
+      <c r="I88" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J88" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5061,7 +5030,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="17" t="s">
+      <c r="A89" s="18" t="s">
         <v>365</v>
       </c>
       <c r="B89" s="8" t="s">
@@ -5081,23 +5050,23 @@
       </c>
       <c r="G89" s="10"/>
       <c r="H89" s="7"/>
-      <c r="I89" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J89" s="11" t="b">
+      <c r="I89" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J89" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K89" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L89" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="17" t="s">
+      <c r="A90" s="18" t="s">
         <v>368</v>
       </c>
       <c r="B90" s="8" t="s">
@@ -5109,7 +5078,7 @@
       <c r="D90" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="E90" s="18" t="s">
+      <c r="E90" s="19" t="s">
         <v>371</v>
       </c>
       <c r="F90" s="7" t="s">
@@ -5117,11 +5086,11 @@
       </c>
       <c r="G90" s="10"/>
       <c r="H90" s="7"/>
-      <c r="I90" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J90" s="11" t="b">
+      <c r="I90" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J90" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5133,7 +5102,7 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="12" t="s">
+      <c r="A91" s="13" t="s">
         <v>373</v>
       </c>
       <c r="B91" s="10" t="s">
@@ -5142,10 +5111,10 @@
       <c r="C91" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="D91" s="13" t="n">
+      <c r="D91" s="14" t="n">
         <v>12</v>
       </c>
-      <c r="E91" s="26" t="s">
+      <c r="E91" s="27" t="s">
         <v>376</v>
       </c>
       <c r="F91" s="7" t="s">
@@ -5155,11 +5124,11 @@
         <v>-1</v>
       </c>
       <c r="H91" s="7"/>
-      <c r="I91" s="11" t="b">
+      <c r="I91" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J91" s="11" t="b">
+      <c r="J91" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5170,7 +5139,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="92" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="92" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="7" t="s">
         <v>377</v>
       </c>
@@ -5191,16 +5160,16 @@
       </c>
       <c r="G92" s="10"/>
       <c r="H92" s="7"/>
-      <c r="I92" s="11" t="b">
+      <c r="I92" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J92" s="11" t="b">
+      <c r="J92" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K92" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L92" s="7" t="s">
         <v>22</v>
@@ -5275,7 +5244,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="13" t="s">
+      <c r="A95" s="14" t="s">
         <v>389</v>
       </c>
       <c r="B95" s="7" t="s">
@@ -5284,7 +5253,7 @@
       <c r="C95" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="D95" s="13" t="n">
+      <c r="D95" s="14" t="n">
         <v>8</v>
       </c>
       <c r="E95" s="9" t="s">
@@ -5329,23 +5298,23 @@
       </c>
       <c r="G96" s="10"/>
       <c r="H96" s="7"/>
-      <c r="I96" s="11" t="b">
+      <c r="I96" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J96" s="11" t="b">
+      <c r="J96" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K96" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L96" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="13" t="s">
+      <c r="A97" s="14" t="s">
         <v>397</v>
       </c>
       <c r="B97" s="7" t="s">
@@ -5354,7 +5323,7 @@
       <c r="C97" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="D97" s="13" t="n">
+      <c r="D97" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E97" s="9" t="s">
@@ -5365,16 +5334,16 @@
       </c>
       <c r="G97" s="10"/>
       <c r="H97" s="7"/>
-      <c r="I97" s="11" t="b">
+      <c r="I97" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J97" s="11" t="b">
+      <c r="J97" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K97" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L97" s="10" t="s">
         <v>176</v>
@@ -5401,16 +5370,16 @@
       </c>
       <c r="G98" s="10"/>
       <c r="H98" s="7"/>
-      <c r="I98" s="11" t="b">
+      <c r="I98" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J98" s="11" t="b">
+      <c r="J98" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K98" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L98" s="7" t="s">
         <v>22</v>
@@ -5437,16 +5406,16 @@
       </c>
       <c r="G99" s="10"/>
       <c r="H99" s="7"/>
-      <c r="I99" s="11" t="b">
+      <c r="I99" s="12" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J99" s="11" t="b">
+      <c r="J99" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K99" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L99" s="7" t="s">
         <v>22</v>
@@ -5478,14 +5447,14 @@
         <v>0</v>
       </c>
       <c r="K100" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L100" s="10" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="13" t="s">
+      <c r="A101" s="14" t="s">
         <v>412</v>
       </c>
       <c r="B101" s="7" t="s">
@@ -5494,7 +5463,7 @@
       <c r="C101" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="D101" s="13" t="n">
+      <c r="D101" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E101" s="9" t="s">
@@ -5505,16 +5474,16 @@
       </c>
       <c r="G101" s="10"/>
       <c r="H101" s="7"/>
-      <c r="I101" s="11" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J101" s="11" t="b">
+      <c r="I101" s="12" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J101" s="12" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K101" s="7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L101" s="10" t="s">
         <v>416</v>
@@ -5554,8 +5523,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" s="14" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="13" t="s">
+    <row r="103" s="15" customFormat="true" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="14" t="s">
         <v>420</v>
       </c>
       <c r="B103" s="7" t="s">
@@ -5564,7 +5533,7 @@
       <c r="C103" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="D103" s="13" t="n">
+      <c r="D103" s="14" t="n">
         <v>4</v>
       </c>
       <c r="E103" s="9" t="s">
@@ -5666,7 +5635,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>